<commit_message>
Enable administrators to manually register new students in the system
Adds a new route, template, and client-side script to allow manual student registration via the `/add_student_form` endpoint and `add_student.html` template.

Replit-Commit-Author: Agent
Replit-Commit-Session-Id: 7e4046e9-32b7-4838-9b98-49020ffa1c80
Replit-Commit-Screenshot-Url: https://storage.googleapis.com/screenshot-production-us-central1/3a213c01-649d-4274-bf74-8c5b6c6afe98/2c70a6ad-29dc-4028-84d9-9d6210aa780c.jpg
</commit_message>
<xml_diff>
--- a/students.xlsx
+++ b/students.xlsx
@@ -550,7 +550,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:C539"/>
+  <dimension ref="A1:C540"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A368" workbookViewId="0">
       <selection activeCell="H411" sqref="H411"/>
@@ -7574,6 +7574,23 @@
         <v>201</v>
       </c>
     </row>
+    <row r="540">
+      <c r="A540" t="inlineStr">
+        <is>
+          <t>10701</t>
+        </is>
+      </c>
+      <c r="B540" t="inlineStr">
+        <is>
+          <t>한가람</t>
+        </is>
+      </c>
+      <c r="C540" t="inlineStr">
+        <is>
+          <t>600</t>
+        </is>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
Improve student data loading and enhance the new student registration process
Reduce cache time to 30 seconds and refine the "add_student.html" template.

Replit-Commit-Author: Agent
Replit-Commit-Session-Id: 7e4046e9-32b7-4838-9b98-49020ffa1c80
Replit-Commit-Screenshot-Url: https://storage.googleapis.com/screenshot-production-us-central1/3a213c01-649d-4274-bf74-8c5b6c6afe98/b094a9a0-0c96-46fa-9a20-85aa72dc8e9b.jpg
</commit_message>
<xml_diff>
--- a/students.xlsx
+++ b/students.xlsx
@@ -550,7 +550,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:C540"/>
+  <dimension ref="A1:C541"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A368" workbookViewId="0">
       <selection activeCell="H411" sqref="H411"/>
@@ -7575,19 +7575,36 @@
       </c>
     </row>
     <row r="540">
-      <c r="A540" t="inlineStr">
+      <c r="A540" s="0" t="inlineStr">
         <is>
           <t>10701</t>
         </is>
       </c>
-      <c r="B540" t="inlineStr">
+      <c r="B540" s="0" t="inlineStr">
         <is>
           <t>한가람</t>
         </is>
       </c>
-      <c r="C540" t="inlineStr">
+      <c r="C540" s="0" t="inlineStr">
         <is>
           <t>600</t>
+        </is>
+      </c>
+    </row>
+    <row r="541">
+      <c r="A541" t="inlineStr">
+        <is>
+          <t>10702</t>
+        </is>
+      </c>
+      <c r="B541" t="inlineStr">
+        <is>
+          <t>김은영</t>
+        </is>
+      </c>
+      <c r="C541" t="inlineStr">
+        <is>
+          <t>601</t>
         </is>
       </c>
     </row>

</xml_diff>

<commit_message>
Update student list immediately after adding new students to the system
Refactors student data loading with forced cache reload after adding a new student, and fixes the seat column lookup.

Replit-Commit-Author: Agent
Replit-Commit-Session-Id: 7e4046e9-32b7-4838-9b98-49020ffa1c80
Replit-Commit-Screenshot-Url: https://storage.googleapis.com/screenshot-production-us-central1/3a213c01-649d-4274-bf74-8c5b6c6afe98/ed373961-ecf2-476c-8975-3c66652abdf3.jpg
</commit_message>
<xml_diff>
--- a/students.xlsx
+++ b/students.xlsx
@@ -550,7 +550,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:C541"/>
+  <dimension ref="A1:C542"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A368" workbookViewId="0">
       <selection activeCell="H411" sqref="H411"/>
@@ -7592,19 +7592,36 @@
       </c>
     </row>
     <row r="541">
-      <c r="A541" t="inlineStr">
+      <c r="A541" s="0" t="inlineStr">
         <is>
           <t>10702</t>
         </is>
       </c>
-      <c r="B541" t="inlineStr">
+      <c r="B541" s="0" t="inlineStr">
         <is>
           <t>김은영</t>
         </is>
       </c>
-      <c r="C541" t="inlineStr">
+      <c r="C541" s="0" t="inlineStr">
         <is>
           <t>601</t>
+        </is>
+      </c>
+    </row>
+    <row r="542">
+      <c r="A542" t="inlineStr">
+        <is>
+          <t>10703</t>
+        </is>
+      </c>
+      <c r="B542" t="inlineStr">
+        <is>
+          <t>한가람</t>
+        </is>
+      </c>
+      <c r="C542" t="inlineStr">
+        <is>
+          <t>602</t>
         </is>
       </c>
     </row>

</xml_diff>

<commit_message>
Make the admin page return to the period view for easier navigation
Changes the return URL in admin templates to always redirect to 'by_period' view.

Replit-Commit-Author: Agent
Replit-Commit-Session-Id: 7e4046e9-32b7-4838-9b98-49020ffa1c80
Replit-Commit-Screenshot-Url: https://storage.googleapis.com/screenshot-production-us-central1/3a213c01-649d-4274-bf74-8c5b6c6afe98/859165c5-5c62-4c16-be48-95fdda20cb5b.jpg
</commit_message>
<xml_diff>
--- a/students.xlsx
+++ b/students.xlsx
@@ -7580,38 +7580,14 @@
       <c r="C540" s="0" t="n"/>
     </row>
     <row r="541">
-      <c r="A541" s="0" t="inlineStr">
-        <is>
-          <t>10702</t>
-        </is>
-      </c>
-      <c r="B541" s="0" t="inlineStr">
-        <is>
-          <t>김은영</t>
-        </is>
-      </c>
-      <c r="C541" s="0" t="inlineStr">
-        <is>
-          <t>601</t>
-        </is>
-      </c>
+      <c r="A541" s="0" t="n"/>
+      <c r="B541" s="0" t="n"/>
+      <c r="C541" s="0" t="n"/>
     </row>
     <row r="542">
-      <c r="A542" s="0" t="inlineStr">
-        <is>
-          <t>10703</t>
-        </is>
-      </c>
-      <c r="B542" s="0" t="inlineStr">
-        <is>
-          <t>한가람</t>
-        </is>
-      </c>
-      <c r="C542" s="0" t="inlineStr">
-        <is>
-          <t>602</t>
-        </is>
-      </c>
+      <c r="A542" s="0" t="n"/>
+      <c r="B542" s="0" t="n"/>
+      <c r="C542" s="0" t="n"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
Add a button to access the timetable configuration page
Add a new button to the `by_period.html` template that links to the `schedule_settings` route, allowing users to configure timetable settings.

Replit-Commit-Author: Agent
Replit-Commit-Session-Id: 7e4046e9-32b7-4838-9b98-49020ffa1c80
Replit-Commit-Checkpoint-Type: intermediate_checkpoint
Replit-Commit-Event-Id: af4546f3-f56f-4ef9-a96b-8c0c10aa53e5
Replit-Commit-Screenshot-Url: https://storage.googleapis.com/screenshot-production-us-central1/3a213c01-649d-4274-bf74-8c5b6c6afe98/7e4046e9-32b7-4838-9b98-49020ffa1c80/549A2TS
</commit_message>
<xml_diff>
--- a/students.xlsx
+++ b/students.xlsx
@@ -413,7 +413,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:C534"/>
+  <dimension ref="A1:C535"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -9499,6 +9499,23 @@
         </is>
       </c>
     </row>
+    <row r="535">
+      <c r="A535" t="inlineStr">
+        <is>
+          <t>10429</t>
+        </is>
+      </c>
+      <c r="B535" t="inlineStr">
+        <is>
+          <t>김원중</t>
+        </is>
+      </c>
+      <c r="C535" t="inlineStr">
+        <is>
+          <t>282</t>
+        </is>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>